<commit_message>
changes in salary finance bb report password
</commit_message>
<xml_diff>
--- a/salaryfinance_monitoring_sheet.xlsx
+++ b/salaryfinance_monitoring_sheet.xlsx
@@ -470,7 +470,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>35.3078502980345</v>
+        <v>35.10251782531287</v>
       </c>
     </row>
     <row r="8">
@@ -481,7 +481,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>22.57%</t>
+          <t>22.63%</t>
         </is>
       </c>
     </row>
@@ -493,7 +493,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>8.22%</t>
+          <t>8.08%</t>
         </is>
       </c>
     </row>
@@ -517,7 +517,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>28.95%</t>
+          <t>28.78%</t>
         </is>
       </c>
     </row>
@@ -529,7 +529,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>6.61%</t>
+          <t>6.79%</t>
         </is>
       </c>
     </row>
@@ -541,7 +541,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>0.27%</t>
+          <t>0.40%</t>
         </is>
       </c>
     </row>
@@ -565,7 +565,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>3.48%</t>
+          <t>3.51%</t>
         </is>
       </c>
     </row>
@@ -577,7 +577,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>2.48%</t>
+          <t>2.46%</t>
         </is>
       </c>
     </row>
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>25037522.2</v>
+        <v>23572221.57</v>
       </c>
     </row>
     <row r="20">
@@ -608,7 +608,7 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>4800850.54</v>
+        <v>8904762.379999999</v>
       </c>
     </row>
     <row r="21">
@@ -619,7 +619,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>1.52%</t>
+          <t>1.50%</t>
         </is>
       </c>
     </row>
@@ -631,7 +631,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>0.60%</t>
+          <t>0.64%</t>
         </is>
       </c>
     </row>
@@ -643,7 +643,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>8.27%</t>
+          <t>8.38%</t>
         </is>
       </c>
     </row>
@@ -654,7 +654,7 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>712845</v>
+        <v>720345</v>
       </c>
     </row>
     <row r="25">
@@ -672,7 +672,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>0.60%</t>
+          <t>0.64%</t>
         </is>
       </c>
     </row>
@@ -683,7 +683,7 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>95046000</v>
+        <v>96046000</v>
       </c>
     </row>
     <row r="28">
@@ -716,7 +716,7 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>110475013.6000005</v>
+        <v>111282723.5587123</v>
       </c>
     </row>
     <row r="34">
@@ -733,7 +733,7 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>3610346.07</v>
+        <v>5245393.65</v>
       </c>
     </row>
     <row r="36">
@@ -743,7 +743,7 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>1180433.52</v>
+        <v>1125255.9</v>
       </c>
     </row>
     <row r="37">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>96046000</v>
+        <v>98468000</v>
       </c>
     </row>
     <row r="38">
@@ -763,7 +763,7 @@
         </is>
       </c>
       <c r="B38" t="n">
-        <v>11860000</v>
+        <v>12160000</v>
       </c>
     </row>
     <row r="39">
@@ -773,7 +773,7 @@
         </is>
       </c>
       <c r="B39" t="n">
-        <v>7359793.190000519</v>
+        <v>7025373.108712301</v>
       </c>
     </row>
     <row r="40">
@@ -783,7 +783,7 @@
         </is>
       </c>
       <c r="B40" t="n">
-        <v>5730000</v>
+        <v>150000</v>
       </c>
     </row>
     <row r="41">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="B41" t="n">
-        <v>0</v>
+        <v>5730000</v>
       </c>
     </row>
     <row r="42">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="B43" t="n">
-        <v>5730000</v>
+        <v>5880000</v>
       </c>
     </row>
     <row r="44">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4270000</v>
+        <v>4120000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>